<commit_message>
add information for mseResult
</commit_message>
<xml_diff>
--- a/GetMSEBeta/mseResultBak.xlsx
+++ b/GetMSEBeta/mseResultBak.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\niujie\GetSene\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\lindinan\ansys\GetMSEBeta\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26610" windowHeight="13965" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="26610" windowHeight="13965"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,19 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sene</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>seneNoDama</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -404,10 +391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -415,15 +402,9 @@
     <col min="2" max="2" width="12.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -431,25 +412,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>